<commit_message>
added no_database functionality for emma_backend.py, started working on research table parsing.
</commit_message>
<xml_diff>
--- a/emma_backend/research/participants/Participant_Table.xlsx
+++ b/emma_backend/research/participants/Participant_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Gerontechnology\emma_backend\research\participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE745AD2-04C2-4ED9-8CB3-ECFB2A7F4215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D56D8B-105C-4034-92F1-DB37FF5D99D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1920" windowWidth="22080" windowHeight="8976" xr2:uid="{67EADD54-F8D8-4F48-A951-41E9FAD070FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67EADD54-F8D8-4F48-A951-41E9FAD070FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>BB</t>
   </si>
@@ -201,99 +201,6 @@
   </si>
   <si>
     <t>bb055</t>
-  </si>
-  <si>
-    <t>bb120</t>
-  </si>
-  <si>
-    <t>bb427</t>
-  </si>
-  <si>
-    <t>bb449</t>
-  </si>
-  <si>
-    <t>bb474</t>
-  </si>
-  <si>
-    <t>bb504</t>
-  </si>
-  <si>
-    <t>bb510</t>
-  </si>
-  <si>
-    <t>bb516</t>
-  </si>
-  <si>
-    <t>bb544</t>
-  </si>
-  <si>
-    <t>bb688</t>
-  </si>
-  <si>
-    <t>bb706</t>
-  </si>
-  <si>
-    <t>bb732</t>
-  </si>
-  <si>
-    <t>bb772</t>
-  </si>
-  <si>
-    <t>bb804</t>
-  </si>
-  <si>
-    <t>bb830</t>
-  </si>
-  <si>
-    <t>bb908</t>
-  </si>
-  <si>
-    <t>bb021</t>
-  </si>
-  <si>
-    <t>bb221</t>
-  </si>
-  <si>
-    <t>bb397</t>
-  </si>
-  <si>
-    <t>bb403</t>
-  </si>
-  <si>
-    <t>bb543</t>
-  </si>
-  <si>
-    <t>bb653</t>
-  </si>
-  <si>
-    <t>bb707</t>
-  </si>
-  <si>
-    <t>bb730</t>
-  </si>
-  <si>
-    <t>bb907</t>
-  </si>
-  <si>
-    <t>bb953</t>
-  </si>
-  <si>
-    <t>bb1090</t>
-  </si>
-  <si>
-    <t>bb1103</t>
-  </si>
-  <si>
-    <t>bb1115</t>
-  </si>
-  <si>
-    <t>bb381</t>
-  </si>
-  <si>
-    <t>bb765</t>
-  </si>
-  <si>
-    <t>bb1002</t>
   </si>
   <si>
     <t>participant_id</t>
@@ -669,29 +576,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6D9D42-CCFA-D947-B448-8AFCAD7E855A}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E86" sqref="A55:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1593,527 +1500,6 @@
       </c>
       <c r="E54">
         <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>189</v>
-      </c>
-      <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>190</v>
-      </c>
-      <c r="B56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>191</v>
-      </c>
-      <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>192</v>
-      </c>
-      <c r="B58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>193</v>
-      </c>
-      <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>194</v>
-      </c>
-      <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>195</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>196</v>
-      </c>
-      <c r="B62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>197</v>
-      </c>
-      <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>198</v>
-      </c>
-      <c r="B64" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>199</v>
-      </c>
-      <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>200</v>
-      </c>
-      <c r="B66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>201</v>
-      </c>
-      <c r="B67" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>202</v>
-      </c>
-      <c r="B68" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>203</v>
-      </c>
-      <c r="B69" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>2</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>204</v>
-      </c>
-      <c r="B70" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>2</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>205</v>
-      </c>
-      <c r="B71" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>2</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>206</v>
-      </c>
-      <c r="B72" t="s">
-        <v>72</v>
-      </c>
-      <c r="C72" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <v>2</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>207</v>
-      </c>
-      <c r="B73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" t="s">
-        <v>0</v>
-      </c>
-      <c r="D73">
-        <v>2</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>208</v>
-      </c>
-      <c r="B74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>209</v>
-      </c>
-      <c r="B75" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75">
-        <v>2</v>
-      </c>
-      <c r="E75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>210</v>
-      </c>
-      <c r="B76" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>211</v>
-      </c>
-      <c r="B77" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>2</v>
-      </c>
-      <c r="E77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>212</v>
-      </c>
-      <c r="B78" t="s">
-        <v>78</v>
-      </c>
-      <c r="C78" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>2</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>213</v>
-      </c>
-      <c r="B79" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>2</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>214</v>
-      </c>
-      <c r="B80" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>2</v>
-      </c>
-      <c r="E80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>215</v>
-      </c>
-      <c r="B81" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81">
-        <v>2</v>
-      </c>
-      <c r="E81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>216</v>
-      </c>
-      <c r="B82" t="s">
-        <v>82</v>
-      </c>
-      <c r="C82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>2</v>
-      </c>
-      <c r="E82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>217</v>
-      </c>
-      <c r="B83" t="s">
-        <v>83</v>
-      </c>
-      <c r="C83" t="s">
-        <v>0</v>
-      </c>
-      <c r="D83">
-        <v>2</v>
-      </c>
-      <c r="E83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>218</v>
-      </c>
-      <c r="B84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" t="s">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>2</v>
-      </c>
-      <c r="E84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>222</v>
-      </c>
-      <c r="B85" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>